<commit_message>
Run notebook to update values
</commit_message>
<xml_diff>
--- a/Spacecraft subsystems.xlsx
+++ b/Spacecraft subsystems.xlsx
@@ -443,10 +443,10 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>6.985898666666667</v>
+        <v>14.73134933333333</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>3.076923076923077</v>
+        <v>6.153846153846154</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>

</xml_diff>